<commit_message>
changing firm name Segal Consulting to Segal
</commit_message>
<xml_diff>
--- a/Actuarial Firm Summary.xlsx
+++ b/Actuarial Firm Summary.xlsx
@@ -13,7 +13,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="37">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="36">
   <si>
     <t xml:space="preserve">actuarial_firm_name</t>
   </si>
@@ -82,9 +82,6 @@
   </si>
   <si>
     <t xml:space="preserve">Bolton</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Segal Consulting</t>
   </si>
   <si>
     <t xml:space="preserve">Definiti</t>
@@ -516,13 +513,13 @@
         <v>7</v>
       </c>
       <c r="B5" t="n">
-        <v>642593016460</v>
+        <v>649806185770</v>
       </c>
       <c r="C5" t="n">
-        <v>0.10691513296308</v>
+        <v>0.108115265762705</v>
       </c>
       <c r="D5" t="n">
-        <v>156640205110</v>
+        <v>160198525120</v>
       </c>
     </row>
     <row r="6">
@@ -740,13 +737,13 @@
         <v>23</v>
       </c>
       <c r="B21" t="n">
-        <v>7213169310</v>
+        <v>4179376800</v>
       </c>
       <c r="C21" t="n">
-        <v>0.00120013279962538</v>
+        <v>0.000695368008722558</v>
       </c>
       <c r="D21" t="n">
-        <v>3558320010</v>
+        <v>658566500</v>
       </c>
     </row>
     <row r="22">
@@ -754,13 +751,13 @@
         <v>24</v>
       </c>
       <c r="B22" t="n">
-        <v>4179376800</v>
+        <v>3793100000</v>
       </c>
       <c r="C22" t="n">
-        <v>0.000695368008722558</v>
+        <v>0.000631098970039153</v>
       </c>
       <c r="D22" t="n">
-        <v>658566500</v>
+        <v>-411732000</v>
       </c>
     </row>
     <row r="23">
@@ -768,13 +765,13 @@
         <v>25</v>
       </c>
       <c r="B23" t="n">
-        <v>3793100000</v>
+        <v>3635244300</v>
       </c>
       <c r="C23" t="n">
-        <v>0.000631098970039153</v>
+        <v>0.000604834814154835</v>
       </c>
       <c r="D23" t="n">
-        <v>-411732000</v>
+        <v>363093300</v>
       </c>
     </row>
     <row r="24">
@@ -782,13 +779,13 @@
         <v>26</v>
       </c>
       <c r="B24" t="n">
-        <v>3635244300</v>
+        <v>3518184500</v>
       </c>
       <c r="C24" t="n">
-        <v>0.000604834814154835</v>
+        <v>0.000585358312292772</v>
       </c>
       <c r="D24" t="n">
-        <v>363093300</v>
+        <v>224574200</v>
       </c>
     </row>
     <row r="25">
@@ -796,13 +793,13 @@
         <v>27</v>
       </c>
       <c r="B25" t="n">
-        <v>3518184500</v>
+        <v>2958058800</v>
       </c>
       <c r="C25" t="n">
-        <v>0.000585358312292772</v>
+        <v>0.000492164156493437</v>
       </c>
       <c r="D25" t="n">
-        <v>224574200</v>
+        <v>527705800</v>
       </c>
     </row>
     <row r="26">
@@ -810,13 +807,13 @@
         <v>28</v>
       </c>
       <c r="B26" t="n">
-        <v>2958058800</v>
+        <v>2100049300</v>
       </c>
       <c r="C26" t="n">
-        <v>0.000492164156493437</v>
+        <v>0.000349407859076071</v>
       </c>
       <c r="D26" t="n">
-        <v>527705800</v>
+        <v>316280700</v>
       </c>
     </row>
     <row r="27">
@@ -824,13 +821,13 @@
         <v>29</v>
       </c>
       <c r="B27" t="n">
-        <v>2100049300</v>
+        <v>1918985910</v>
       </c>
       <c r="C27" t="n">
-        <v>0.000349407859076071</v>
+        <v>0.00031928238942307</v>
       </c>
       <c r="D27" t="n">
-        <v>316280700</v>
+        <v>470194990</v>
       </c>
     </row>
     <row r="28">
@@ -838,13 +835,13 @@
         <v>30</v>
       </c>
       <c r="B28" t="n">
-        <v>1918985910</v>
+        <v>1313297900</v>
       </c>
       <c r="C28" t="n">
-        <v>0.00031928238942307</v>
+        <v>0.000218507540545882</v>
       </c>
       <c r="D28" t="n">
-        <v>470194990</v>
+        <v>9753400.00000014</v>
       </c>
     </row>
     <row r="29">
@@ -852,13 +849,13 @@
         <v>31</v>
       </c>
       <c r="B29" t="n">
-        <v>1313297900</v>
+        <v>703817630</v>
       </c>
       <c r="C29" t="n">
-        <v>0.000218507540545882</v>
+        <v>0.000117101732458516</v>
       </c>
       <c r="D29" t="n">
-        <v>9753400.00000014</v>
+        <v>151461190</v>
       </c>
     </row>
     <row r="30">
@@ -866,13 +863,13 @@
         <v>32</v>
       </c>
       <c r="B30" t="n">
-        <v>703817630</v>
+        <v>696707380</v>
       </c>
       <c r="C30" t="n">
-        <v>0.000117101732458516</v>
+        <v>0.000115918723454873</v>
       </c>
       <c r="D30" t="n">
-        <v>151461190</v>
+        <v>-54478500</v>
       </c>
     </row>
     <row r="31">
@@ -880,13 +877,13 @@
         <v>33</v>
       </c>
       <c r="B31" t="n">
-        <v>696707380</v>
+        <v>130922410</v>
       </c>
       <c r="C31" t="n">
-        <v>0.000115918723454873</v>
+        <v>0.0000217829738488423</v>
       </c>
       <c r="D31" t="n">
-        <v>-54478500</v>
+        <v>-1212889.99999998</v>
       </c>
     </row>
     <row r="32">
@@ -894,26 +891,12 @@
         <v>34</v>
       </c>
       <c r="B32" t="n">
-        <v>130922410</v>
+        <v>65543141</v>
       </c>
       <c r="C32" t="n">
-        <v>0.0000217829738488423</v>
+        <v>0.0000109051195007332</v>
       </c>
       <c r="D32" t="n">
-        <v>-1212889.99999998</v>
-      </c>
-    </row>
-    <row r="33">
-      <c r="A33" t="s">
-        <v>35</v>
-      </c>
-      <c r="B33" t="n">
-        <v>65543141</v>
-      </c>
-      <c r="C33" t="n">
-        <v>0.0000109051195007332</v>
-      </c>
-      <c r="D33" t="n">
         <v>1679539</v>
       </c>
     </row>
@@ -992,13 +975,13 @@
         <v>7</v>
       </c>
       <c r="B5" t="n">
-        <v>642593016460</v>
+        <v>649806185770</v>
       </c>
       <c r="C5" t="n">
-        <v>0.10691513296308</v>
+        <v>0.108115265762705</v>
       </c>
       <c r="D5" t="n">
-        <v>156640205110</v>
+        <v>160198525120</v>
       </c>
     </row>
     <row r="6">
@@ -1157,16 +1140,16 @@
     </row>
     <row r="17">
       <c r="A17" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="B17" t="n">
-        <v>114462989079</v>
+        <v>107249819769</v>
       </c>
       <c r="C17" t="n">
-        <v>0.0190444424126334</v>
+        <v>0.017844309613008</v>
       </c>
       <c r="D17" t="n">
-        <v>18615220813</v>
+        <v>15056900803</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
fixing NA firms names
</commit_message>
<xml_diff>
--- a/Actuarial Firm Summary.xlsx
+++ b/Actuarial Firm Summary.xlsx
@@ -6,14 +6,14 @@
     <workbookView xWindow="0" yWindow="0" windowWidth="13125" windowHeight="6105" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
-    <sheet name="Actuarial Firm Summary" sheetId="1" state="visible" r:id="rId1"/>
-    <sheet name="Actuarial Firm Summary 2" sheetId="2" state="visible" r:id="rId2"/>
+    <sheet name="Actuarial Firm Summary16_21" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet name="Actuarial Firm Summary 3_2021" sheetId="2" state="visible" r:id="rId2"/>
   </sheets>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="48">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="50">
   <si>
     <t xml:space="preserve">actuarial_firm_name</t>
   </si>
@@ -45,45 +45,51 @@
     <t xml:space="preserve">CalPERS</t>
   </si>
   <si>
+    <t xml:space="preserve">Scott Terando</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Conduent (formerly Buck and/or Xerox)</t>
+  </si>
+  <si>
     <t xml:space="preserve">Cheiron</t>
   </si>
   <si>
     <t xml:space="preserve">New York City Office of the Actuary</t>
   </si>
   <si>
-    <t xml:space="preserve">Conduent</t>
-  </si>
-  <si>
     <t xml:space="preserve">New York State and Local Retirement Systems' Actuary</t>
   </si>
   <si>
-    <t xml:space="preserve">Buck</t>
+    <t xml:space="preserve">Internal Actuarial Services</t>
+  </si>
+  <si>
+    <t xml:space="preserve">New York State And Local Retirement Systems' Actuary</t>
   </si>
   <si>
     <t xml:space="preserve">Nystrs Office Of The Actuary</t>
   </si>
   <si>
-    <t xml:space="preserve">Public Employee Retirement Administration Commission</t>
-  </si>
-  <si>
     <t xml:space="preserve">Foster &amp; Foster</t>
   </si>
   <si>
+    <t xml:space="preserve">Office of The State Actuary - Washington</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Perac</t>
+  </si>
+  <si>
     <t xml:space="preserve">Pwc</t>
   </si>
   <si>
     <t xml:space="preserve">Korn Ferry Hay Group</t>
   </si>
   <si>
-    <t xml:space="preserve">Office Of The State Actuary - Washington</t>
+    <t xml:space="preserve">Bryan, Pendleton, Swats &amp; Mcallister, Llc</t>
   </si>
   <si>
     <t xml:space="preserve">USI Consulting Group</t>
   </si>
   <si>
-    <t xml:space="preserve">Office of the State Actuary - Washington</t>
-  </si>
-  <si>
     <t xml:space="preserve">Lousiana Legislative Auditor</t>
   </si>
   <si>
@@ -93,6 +99,9 @@
     <t xml:space="preserve">Actuary South Dakota Retirement System</t>
   </si>
   <si>
+    <t xml:space="preserve">Cbiz</t>
+  </si>
+  <si>
     <t xml:space="preserve">G. S. Curran &amp; Company</t>
   </si>
   <si>
@@ -102,9 +111,6 @@
     <t xml:space="preserve">Bolton</t>
   </si>
   <si>
-    <t xml:space="preserve">Bryan, Pendleton, Swats &amp; Mcallister, Llc</t>
-  </si>
-  <si>
     <t xml:space="preserve">Definiti</t>
   </si>
   <si>
@@ -132,9 +138,6 @@
     <t xml:space="preserve">Mockenhaupt</t>
   </si>
   <si>
-    <t xml:space="preserve">Xerox</t>
-  </si>
-  <si>
     <t xml:space="preserve">Boomershine Consulting Group</t>
   </si>
   <si>
@@ -153,7 +156,10 @@
     <t xml:space="preserve">Principal Financial Group</t>
   </si>
   <si>
-    <t xml:space="preserve">Shdr</t>
+    <t xml:space="preserve">McGriff Employee Benefit Solutions</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Year</t>
   </si>
   <si>
     <t xml:space="preserve">Others</t>
@@ -516,7 +522,7 @@
         <v>1448217745970</v>
       </c>
       <c r="D2" t="n">
-        <v>0.151607537215197</v>
+        <v>0.132657780249413</v>
       </c>
       <c r="E2" t="n">
         <v>261234414860</v>
@@ -530,13 +536,13 @@
         <v>2016</v>
       </c>
       <c r="C3" t="n">
-        <v>996526878810</v>
+        <v>1145910773040</v>
       </c>
       <c r="D3" t="n">
-        <v>0.104322009784474</v>
+        <v>0.104966245537585</v>
       </c>
       <c r="E3" t="n">
-        <v>311089564460</v>
+        <v>353013780172</v>
       </c>
     </row>
     <row r="4">
@@ -550,7 +556,7 @@
         <v>901490366670</v>
       </c>
       <c r="D4" t="n">
-        <v>0.0943730559126122</v>
+        <v>0.0825771616812854</v>
       </c>
       <c r="E4" t="n">
         <v>154718673140</v>
@@ -567,7 +573,7 @@
         <v>791425215550</v>
       </c>
       <c r="D5" t="n">
-        <v>0.0828508200189033</v>
+        <v>0.0724951151996524</v>
       </c>
       <c r="E5" t="n">
         <v>49509898210</v>
@@ -581,47 +587,47 @@
         <v>2016</v>
       </c>
       <c r="C6" t="n">
-        <v>683670996000</v>
+        <v>684066156000</v>
       </c>
       <c r="D6" t="n">
-        <v>0.0715705053728628</v>
+        <v>0.062660948639272</v>
       </c>
       <c r="E6" t="n">
-        <v>177433608700</v>
+        <v>177510694110</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="B7" t="n">
-        <v>2021</v>
+        <v>2016</v>
       </c>
       <c r="C7" t="n">
-        <v>649806185770</v>
+        <v>668830779530</v>
       </c>
       <c r="D7" t="n">
-        <v>0.0680253475459287</v>
+        <v>0.0612653772692909</v>
       </c>
       <c r="E7" t="n">
-        <v>160198525120</v>
+        <v>235119454970</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="s">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="B8" t="n">
-        <v>2016</v>
+        <v>2021</v>
       </c>
       <c r="C8" t="n">
-        <v>635354555300</v>
+        <v>649806185770</v>
       </c>
       <c r="D8" t="n">
-        <v>0.0665124700035856</v>
+        <v>0.0595227108882364</v>
       </c>
       <c r="E8" t="n">
-        <v>219302805490</v>
+        <v>160198525120</v>
       </c>
     </row>
     <row r="9">
@@ -635,7 +641,7 @@
         <v>587976000000</v>
       </c>
       <c r="D9" t="n">
-        <v>0.06155261772596</v>
+        <v>0.0538590216954464</v>
       </c>
       <c r="E9" t="n">
         <v>110653248000</v>
@@ -649,13 +655,13 @@
         <v>2016</v>
       </c>
       <c r="C10" t="n">
-        <v>492881376200</v>
+        <v>510644048790</v>
       </c>
       <c r="D10" t="n">
-        <v>0.0515975804003628</v>
+        <v>0.0467753597126944</v>
       </c>
       <c r="E10" t="n">
-        <v>185530941400</v>
+        <v>193838029190</v>
       </c>
     </row>
     <row r="11">
@@ -663,16 +669,16 @@
         <v>10</v>
       </c>
       <c r="B11" t="n">
-        <v>2021</v>
+        <v>2016</v>
       </c>
       <c r="C11" t="n">
-        <v>357816501213</v>
+        <v>436703008000</v>
       </c>
       <c r="D11" t="n">
-        <v>0.0374582335251852</v>
+        <v>0.0400023075471426</v>
       </c>
       <c r="E11" t="n">
-        <v>97309179763</v>
+        <v>137999008000</v>
       </c>
     </row>
     <row r="12">
@@ -680,16 +686,16 @@
         <v>11</v>
       </c>
       <c r="B12" t="n">
-        <v>2021</v>
+        <v>2016</v>
       </c>
       <c r="C12" t="n">
-        <v>248994048500</v>
+        <v>385162844740</v>
       </c>
       <c r="D12" t="n">
-        <v>0.0260660902542955</v>
+        <v>0.035281191768255</v>
       </c>
       <c r="E12" t="n">
-        <v>7493808500</v>
+        <v>132914565260</v>
       </c>
     </row>
     <row r="13">
@@ -697,16 +703,16 @@
         <v>12</v>
       </c>
       <c r="B13" t="n">
-        <v>2016</v>
+        <v>2021</v>
       </c>
       <c r="C13" t="n">
-        <v>248938314280</v>
+        <v>357816501213</v>
       </c>
       <c r="D13" t="n">
-        <v>0.0260602556842826</v>
+        <v>0.0327762471628429</v>
       </c>
       <c r="E13" t="n">
-        <v>70921861500</v>
+        <v>97309179763</v>
       </c>
     </row>
     <row r="14">
@@ -717,13 +723,13 @@
         <v>2021</v>
       </c>
       <c r="C14" t="n">
-        <v>231904000000</v>
+        <v>248994048500</v>
       </c>
       <c r="D14" t="n">
-        <v>0.0242770083491861</v>
+        <v>0.0228080327431707</v>
       </c>
       <c r="E14" t="n">
-        <v>-28177076000</v>
+        <v>7493808500</v>
       </c>
     </row>
     <row r="15">
@@ -734,13 +740,13 @@
         <v>2021</v>
       </c>
       <c r="C15" t="n">
-        <v>161404206940</v>
+        <v>231904000000</v>
       </c>
       <c r="D15" t="n">
-        <v>0.0168966955269255</v>
+        <v>0.0212425720901207</v>
       </c>
       <c r="E15" t="n">
-        <v>45675353140</v>
+        <v>-28177076000</v>
       </c>
     </row>
     <row r="16">
@@ -748,67 +754,67 @@
         <v>15</v>
       </c>
       <c r="B16" t="n">
-        <v>2021</v>
+        <v>2016</v>
       </c>
       <c r="C16" t="n">
-        <v>131077400000</v>
+        <v>221998704000</v>
       </c>
       <c r="D16" t="n">
-        <v>0.0137219156814441</v>
+        <v>0.0203352398994125</v>
       </c>
       <c r="E16" t="n">
-        <v>-17071064000</v>
+        <v>75081150000</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="B17" t="n">
         <v>2016</v>
       </c>
       <c r="C17" t="n">
-        <v>109305104000</v>
+        <v>202866000000</v>
       </c>
       <c r="D17" t="n">
-        <v>0.0114426699083097</v>
+        <v>0.0185826705431317</v>
       </c>
       <c r="E17" t="n">
-        <v>1798960000</v>
+        <v>19225796000</v>
       </c>
     </row>
     <row r="18">
       <c r="A18" t="s">
-        <v>16</v>
+        <v>11</v>
       </c>
       <c r="B18" t="n">
         <v>2021</v>
       </c>
       <c r="C18" t="n">
-        <v>104534296000</v>
+        <v>161404206940</v>
       </c>
       <c r="D18" t="n">
-        <v>0.0109432350316005</v>
+        <v>0.0147847406753299</v>
       </c>
       <c r="E18" t="n">
-        <v>31406700000</v>
+        <v>45675353140</v>
       </c>
     </row>
     <row r="19">
       <c r="A19" t="s">
-        <v>10</v>
+        <v>17</v>
       </c>
       <c r="B19" t="n">
-        <v>2016</v>
+        <v>2021</v>
       </c>
       <c r="C19" t="n">
-        <v>83016309898</v>
+        <v>131077400000</v>
       </c>
       <c r="D19" t="n">
-        <v>0.0086906118415912</v>
+        <v>0.0120067834918138</v>
       </c>
       <c r="E19" t="n">
-        <v>18663664808</v>
+        <v>-17071064000</v>
       </c>
     </row>
     <row r="20">
@@ -816,33 +822,33 @@
         <v>17</v>
       </c>
       <c r="B20" t="n">
-        <v>2021</v>
+        <v>2016</v>
       </c>
       <c r="C20" t="n">
-        <v>78963501600</v>
+        <v>109305104000</v>
       </c>
       <c r="D20" t="n">
-        <v>0.00826634119128678</v>
+        <v>0.0100124256224047</v>
       </c>
       <c r="E20" t="n">
-        <v>20951535600</v>
+        <v>1798960000</v>
       </c>
     </row>
     <row r="21">
       <c r="A21" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="B21" t="n">
-        <v>2016</v>
+        <v>2021</v>
       </c>
       <c r="C21" t="n">
-        <v>64963232000</v>
+        <v>104534296000</v>
       </c>
       <c r="D21" t="n">
-        <v>0.00680071463042515</v>
+        <v>0.00957541620097116</v>
       </c>
       <c r="E21" t="n">
-        <v>12781431200</v>
+        <v>31406700000</v>
       </c>
     </row>
     <row r="22">
@@ -853,13 +859,13 @@
         <v>2021</v>
       </c>
       <c r="C22" t="n">
-        <v>59395150000</v>
+        <v>98364489600</v>
       </c>
       <c r="D22" t="n">
-        <v>0.00621781665021371</v>
+        <v>0.00901025752654515</v>
       </c>
       <c r="E22" t="n">
-        <v>2321468000</v>
+        <v>28795731600</v>
       </c>
     </row>
     <row r="23">
@@ -870,47 +876,47 @@
         <v>2021</v>
       </c>
       <c r="C23" t="n">
-        <v>52926848000</v>
+        <v>97128000000</v>
       </c>
       <c r="D23" t="n">
-        <v>0.00554067860318107</v>
+        <v>0.00889699419574152</v>
       </c>
       <c r="E23" t="n">
-        <v>12695832000</v>
+        <v>-13019696000</v>
       </c>
     </row>
     <row r="24">
       <c r="A24" t="s">
-        <v>20</v>
+        <v>12</v>
       </c>
       <c r="B24" t="n">
-        <v>2021</v>
+        <v>2016</v>
       </c>
       <c r="C24" t="n">
-        <v>52039000000</v>
+        <v>94665352398</v>
       </c>
       <c r="D24" t="n">
-        <v>0.00544773370654795</v>
+        <v>0.00867141391589276</v>
       </c>
       <c r="E24" t="n">
-        <v>-7024552000</v>
+        <v>25489705898</v>
       </c>
     </row>
     <row r="25">
       <c r="A25" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="B25" t="n">
         <v>2016</v>
       </c>
       <c r="C25" t="n">
-        <v>47518964000</v>
+        <v>83529088000</v>
       </c>
       <c r="D25" t="n">
-        <v>0.0049745510460047</v>
+        <v>0.00765132414042895</v>
       </c>
       <c r="E25" t="n">
-        <v>21131076000</v>
+        <v>34615860000</v>
       </c>
     </row>
     <row r="26">
@@ -918,118 +924,118 @@
         <v>21</v>
       </c>
       <c r="B26" t="n">
-        <v>2021</v>
+        <v>2016</v>
       </c>
       <c r="C26" t="n">
-        <v>45250140000</v>
+        <v>64963232000</v>
       </c>
       <c r="D26" t="n">
-        <v>0.00473703785437871</v>
+        <v>0.00595067846594813</v>
       </c>
       <c r="E26" t="n">
-        <v>13589248000</v>
+        <v>12781431200</v>
       </c>
     </row>
     <row r="27">
       <c r="A27" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
       <c r="B27" t="n">
-        <v>2021</v>
+        <v>2016</v>
       </c>
       <c r="C27" t="n">
-        <v>45089000000</v>
+        <v>61139000000</v>
       </c>
       <c r="D27" t="n">
-        <v>0.00472016881751264</v>
+        <v>0.00560037608242156</v>
       </c>
       <c r="E27" t="n">
-        <v>-5995144000</v>
+        <v>5427847000</v>
       </c>
     </row>
     <row r="28">
       <c r="A28" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="B28" t="n">
-        <v>2016</v>
+        <v>2021</v>
       </c>
       <c r="C28" t="n">
-        <v>34759000000</v>
+        <v>59395150000</v>
       </c>
       <c r="D28" t="n">
-        <v>0.00363876661553643</v>
+        <v>0.00544063817648049</v>
       </c>
       <c r="E28" t="n">
-        <v>4273948000</v>
+        <v>2321468000</v>
       </c>
     </row>
     <row r="29">
       <c r="A29" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B29" t="n">
-        <v>2016</v>
+        <v>2021</v>
       </c>
       <c r="C29" t="n">
-        <v>29272400000</v>
+        <v>52926848000</v>
       </c>
       <c r="D29" t="n">
-        <v>0.00306439862702116</v>
+        <v>0.00484813709182619</v>
       </c>
       <c r="E29" t="n">
-        <v>11734450000</v>
+        <v>12695832000</v>
       </c>
     </row>
     <row r="30">
       <c r="A30" t="s">
-        <v>14</v>
+        <v>22</v>
       </c>
       <c r="B30" t="n">
         <v>2016</v>
       </c>
       <c r="C30" t="n">
-        <v>28999342500</v>
+        <v>47518964000</v>
       </c>
       <c r="D30" t="n">
-        <v>0.00303581344001573</v>
+        <v>0.00435277105361637</v>
       </c>
       <c r="E30" t="n">
-        <v>9830645100</v>
+        <v>21131076000</v>
       </c>
     </row>
     <row r="31">
       <c r="A31" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B31" t="n">
         <v>2016</v>
       </c>
       <c r="C31" t="n">
-        <v>24886090100</v>
+        <v>45894705000</v>
       </c>
       <c r="D31" t="n">
-        <v>0.00260521516289627</v>
+        <v>0.00420398776872034</v>
       </c>
       <c r="E31" t="n">
-        <v>12787232600</v>
+        <v>2588496000</v>
       </c>
     </row>
     <row r="32">
       <c r="A32" t="s">
-        <v>17</v>
+        <v>24</v>
       </c>
       <c r="B32" t="n">
-        <v>2016</v>
+        <v>2021</v>
       </c>
       <c r="C32" t="n">
-        <v>22339367550</v>
+        <v>45250140000</v>
       </c>
       <c r="D32" t="n">
-        <v>0.00233860999606254</v>
+        <v>0.00414494515419335</v>
       </c>
       <c r="E32" t="n">
-        <v>9039656310</v>
+        <v>13589248000</v>
       </c>
     </row>
     <row r="33">
@@ -1037,16 +1043,16 @@
         <v>25</v>
       </c>
       <c r="B33" t="n">
-        <v>2021</v>
+        <v>2016</v>
       </c>
       <c r="C33" t="n">
-        <v>13865352000</v>
+        <v>29272400000</v>
       </c>
       <c r="D33" t="n">
-        <v>0.00145150263155618</v>
+        <v>0.0026813727544624</v>
       </c>
       <c r="E33" t="n">
-        <v>-766847000</v>
+        <v>11734450000</v>
       </c>
     </row>
     <row r="34">
@@ -1054,84 +1060,84 @@
         <v>26</v>
       </c>
       <c r="B34" t="n">
-        <v>2021</v>
+        <v>2016</v>
       </c>
       <c r="C34" t="n">
-        <v>12346287600</v>
+        <v>24886090100</v>
       </c>
       <c r="D34" t="n">
-        <v>0.0012924784701715</v>
+        <v>0.00227958363370398</v>
       </c>
       <c r="E34" t="n">
-        <v>665358900</v>
+        <v>12787232600</v>
       </c>
     </row>
     <row r="35">
       <c r="A35" t="s">
-        <v>27</v>
+        <v>18</v>
       </c>
       <c r="B35" t="n">
         <v>2016</v>
       </c>
       <c r="C35" t="n">
-        <v>10851252000</v>
+        <v>22339367550</v>
       </c>
       <c r="D35" t="n">
-        <v>0.00113596977802505</v>
+        <v>0.00204630202854879</v>
       </c>
       <c r="E35" t="n">
-        <v>337790000</v>
+        <v>9039656310</v>
       </c>
     </row>
     <row r="36">
       <c r="A36" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B36" t="n">
         <v>2021</v>
       </c>
       <c r="C36" t="n">
-        <v>10713525520</v>
+        <v>13865352000</v>
       </c>
       <c r="D36" t="n">
-        <v>0.00112155179944399</v>
+        <v>0.00127007614967788</v>
       </c>
       <c r="E36" t="n">
-        <v>-693364263</v>
+        <v>-766847000</v>
       </c>
     </row>
     <row r="37">
       <c r="A37" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B37" t="n">
         <v>2016</v>
       </c>
       <c r="C37" t="n">
-        <v>8919093000</v>
+        <v>13679861000</v>
       </c>
       <c r="D37" t="n">
-        <v>0.000933700562423103</v>
+        <v>0.00125308504154879</v>
       </c>
       <c r="E37" t="n">
-        <v>251428000</v>
+        <v>5206363000</v>
       </c>
     </row>
     <row r="38">
       <c r="A38" t="s">
-        <v>26</v>
+        <v>29</v>
       </c>
       <c r="B38" t="n">
-        <v>2016</v>
+        <v>2021</v>
       </c>
       <c r="C38" t="n">
-        <v>6567489400</v>
+        <v>12346287600</v>
       </c>
       <c r="D38" t="n">
-        <v>0.000687521539072164</v>
+        <v>0.001130928765301</v>
       </c>
       <c r="E38" t="n">
-        <v>2161742890</v>
+        <v>665358900</v>
       </c>
     </row>
     <row r="39">
@@ -1139,16 +1145,16 @@
         <v>30</v>
       </c>
       <c r="B39" t="n">
-        <v>2021</v>
+        <v>2016</v>
       </c>
       <c r="C39" t="n">
-        <v>4179376800</v>
+        <v>10851252000</v>
       </c>
       <c r="D39" t="n">
-        <v>0.000437520549313486</v>
+        <v>0.00099398243617215</v>
       </c>
       <c r="E39" t="n">
-        <v>658566500</v>
+        <v>337790000</v>
       </c>
     </row>
     <row r="40">
@@ -1159,149 +1165,149 @@
         <v>2021</v>
       </c>
       <c r="C40" t="n">
-        <v>3793100000</v>
+        <v>10713525520</v>
       </c>
       <c r="D40" t="n">
-        <v>0.000397082932460405</v>
+        <v>0.00098136659220172</v>
       </c>
       <c r="E40" t="n">
-        <v>-411732000</v>
+        <v>-693364263</v>
       </c>
     </row>
     <row r="41">
       <c r="A41" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
       <c r="B41" t="n">
-        <v>2021</v>
+        <v>2016</v>
       </c>
       <c r="C41" t="n">
-        <v>3635244300</v>
+        <v>10297901900</v>
       </c>
       <c r="D41" t="n">
-        <v>0.000380557714495788</v>
+        <v>0.00094329517165612</v>
       </c>
       <c r="E41" t="n">
-        <v>363093300</v>
+        <v>2302482390</v>
       </c>
     </row>
     <row r="42">
       <c r="A42" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B42" t="n">
         <v>2021</v>
       </c>
       <c r="C42" t="n">
-        <v>3518184500</v>
+        <v>4179376800</v>
       </c>
       <c r="D42" t="n">
-        <v>0.00036830323961845</v>
+        <v>0.000382833900949436</v>
       </c>
       <c r="E42" t="n">
-        <v>224574200</v>
+        <v>658566500</v>
       </c>
     </row>
     <row r="43">
       <c r="A43" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B43" t="n">
         <v>2021</v>
       </c>
       <c r="C43" t="n">
-        <v>2958058800</v>
+        <v>3793100000</v>
       </c>
       <c r="D43" t="n">
-        <v>0.000309666147134087</v>
+        <v>0.000347450670083469</v>
       </c>
       <c r="E43" t="n">
-        <v>527705800</v>
+        <v>-411732000</v>
       </c>
     </row>
     <row r="44">
       <c r="A44" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B44" t="n">
-        <v>2016</v>
+        <v>2021</v>
       </c>
       <c r="C44" t="n">
-        <v>2904694300</v>
+        <v>3635244300</v>
       </c>
       <c r="D44" t="n">
-        <v>0.000304079652670645</v>
+        <v>0.00033299097517917</v>
       </c>
       <c r="E44" t="n">
-        <v>216467500</v>
+        <v>363093300</v>
       </c>
     </row>
     <row r="45">
       <c r="A45" t="s">
-        <v>33</v>
+        <v>35</v>
       </c>
       <c r="B45" t="n">
-        <v>2016</v>
+        <v>2021</v>
       </c>
       <c r="C45" t="n">
-        <v>2867807300</v>
+        <v>3518184500</v>
       </c>
       <c r="D45" t="n">
-        <v>0.00030021811510779</v>
+        <v>0.000322268213862612</v>
       </c>
       <c r="E45" t="n">
-        <v>625260800</v>
+        <v>224574200</v>
       </c>
     </row>
     <row r="46">
       <c r="A46" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="B46" t="n">
-        <v>2016</v>
+        <v>2021</v>
       </c>
       <c r="C46" t="n">
-        <v>2152521300</v>
+        <v>2958058800</v>
       </c>
       <c r="D46" t="n">
-        <v>0.00022533797421304</v>
+        <v>0.00027096029954557</v>
       </c>
       <c r="E46" t="n">
-        <v>589469300</v>
+        <v>527705800</v>
       </c>
     </row>
     <row r="47">
       <c r="A47" t="s">
-        <v>24</v>
+        <v>37</v>
       </c>
       <c r="B47" t="n">
-        <v>2021</v>
+        <v>2016</v>
       </c>
       <c r="C47" t="n">
-        <v>2100049300</v>
+        <v>2904694300</v>
       </c>
       <c r="D47" t="n">
-        <v>0.000219844911643621</v>
+        <v>0.000266072073217852</v>
       </c>
       <c r="E47" t="n">
-        <v>316280700</v>
+        <v>216467500</v>
       </c>
     </row>
     <row r="48">
       <c r="A48" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="B48" t="n">
-        <v>2021</v>
+        <v>2016</v>
       </c>
       <c r="C48" t="n">
-        <v>1918985910</v>
+        <v>2867807300</v>
       </c>
       <c r="D48" t="n">
-        <v>0.000200890182830139</v>
+        <v>0.000262693197662931</v>
       </c>
       <c r="E48" t="n">
-        <v>470194990</v>
+        <v>625260800</v>
       </c>
     </row>
     <row r="49">
@@ -1312,30 +1318,30 @@
         <v>2016</v>
       </c>
       <c r="C49" t="n">
-        <v>1425378000</v>
+        <v>2152521300</v>
       </c>
       <c r="D49" t="n">
-        <v>0.00014921654480624</v>
+        <v>0.000197172489007392</v>
       </c>
       <c r="E49" t="n">
-        <v>425714000</v>
+        <v>589469300</v>
       </c>
     </row>
     <row r="50">
       <c r="A50" t="s">
-        <v>37</v>
+        <v>26</v>
       </c>
       <c r="B50" t="n">
         <v>2021</v>
       </c>
       <c r="C50" t="n">
-        <v>1313297900</v>
+        <v>2100049300</v>
       </c>
       <c r="D50" t="n">
-        <v>0.000137483372789036</v>
+        <v>0.000192366016317345</v>
       </c>
       <c r="E50" t="n">
-        <v>9753400.00000014</v>
+        <v>316280700</v>
       </c>
     </row>
     <row r="51">
@@ -1343,152 +1349,152 @@
         <v>38</v>
       </c>
       <c r="B51" t="n">
-        <v>2016</v>
+        <v>2021</v>
       </c>
       <c r="C51" t="n">
-        <v>1299809870</v>
+        <v>1918985910</v>
       </c>
       <c r="D51" t="n">
-        <v>0.000136071370335762</v>
+        <v>0.000175780480427681</v>
       </c>
       <c r="E51" t="n">
-        <v>604379950</v>
+        <v>470194990</v>
       </c>
     </row>
     <row r="52">
       <c r="A52" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B52" t="n">
         <v>2016</v>
       </c>
       <c r="C52" t="n">
-        <v>744960000</v>
+        <v>1425378000</v>
       </c>
       <c r="D52" t="n">
-        <v>0.0000779865812569411</v>
+        <v>0.000130565643200083</v>
       </c>
       <c r="E52" t="n">
-        <v>197944870</v>
+        <v>425714000</v>
       </c>
     </row>
     <row r="53">
       <c r="A53" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="B53" t="n">
         <v>2021</v>
       </c>
       <c r="C53" t="n">
-        <v>703817630</v>
+        <v>1313297900</v>
       </c>
       <c r="D53" t="n">
-        <v>0.0000736795677513728</v>
+        <v>0.000120299025961407</v>
       </c>
       <c r="E53" t="n">
-        <v>151461190</v>
+        <v>9753400.00000014</v>
       </c>
     </row>
     <row r="54">
       <c r="A54" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B54" t="n">
-        <v>2021</v>
+        <v>2016</v>
       </c>
       <c r="C54" t="n">
-        <v>696707380</v>
+        <v>1299809870</v>
       </c>
       <c r="D54" t="n">
-        <v>0.0000729352269956515</v>
+        <v>0.000119063512776517</v>
       </c>
       <c r="E54" t="n">
-        <v>-54478500</v>
+        <v>604379950</v>
       </c>
     </row>
     <row r="55">
       <c r="A55" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="B55" t="n">
-        <v>2016</v>
+        <v>2021</v>
       </c>
       <c r="C55" t="n">
-        <v>609079630</v>
+        <v>703817630</v>
       </c>
       <c r="D55" t="n">
-        <v>0.000063761863800664</v>
+        <v>0.0000644701977696499</v>
       </c>
       <c r="E55" t="n">
-        <v>255469630</v>
+        <v>151461190</v>
       </c>
     </row>
     <row r="56">
       <c r="A56" t="s">
-        <v>40</v>
+        <v>42</v>
       </c>
       <c r="B56" t="n">
-        <v>2016</v>
+        <v>2021</v>
       </c>
       <c r="C56" t="n">
-        <v>561973000</v>
+        <v>696707380</v>
       </c>
       <c r="D56" t="n">
-        <v>0.0000588304781850126</v>
+        <v>0.0000638188937895384</v>
       </c>
       <c r="E56" t="n">
-        <v>161951970</v>
+        <v>-54478500</v>
       </c>
     </row>
     <row r="57">
       <c r="A57" t="s">
-        <v>41</v>
+        <v>43</v>
       </c>
       <c r="B57" t="n">
         <v>2016</v>
       </c>
       <c r="C57" t="n">
-        <v>545044060</v>
+        <v>609079630</v>
       </c>
       <c r="D57" t="n">
-        <v>0.000057058262019173</v>
+        <v>0.0000557921292815089</v>
       </c>
       <c r="E57" t="n">
-        <v>56796680</v>
+        <v>255469630</v>
       </c>
     </row>
     <row r="58">
       <c r="A58" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="B58" t="n">
-        <v>2021</v>
+        <v>2016</v>
       </c>
       <c r="C58" t="n">
-        <v>130922410</v>
+        <v>561973000</v>
       </c>
       <c r="D58" t="n">
-        <v>0.0000137056904609906</v>
+        <v>0.0000514771283168958</v>
       </c>
       <c r="E58" t="n">
-        <v>-1212889.99999998</v>
+        <v>161951970</v>
       </c>
     </row>
     <row r="59">
       <c r="A59" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B59" t="n">
         <v>2016</v>
       </c>
       <c r="C59" t="n">
-        <v>96540609</v>
+        <v>545044060</v>
       </c>
       <c r="D59" t="n">
-        <v>0.000010106411147408</v>
+        <v>0.0000499264253175541</v>
       </c>
       <c r="E59" t="n">
-        <v>9793851</v>
+        <v>56796680</v>
       </c>
     </row>
     <row r="60">
@@ -1496,50 +1502,50 @@
         <v>44</v>
       </c>
       <c r="B60" t="n">
-        <v>2016</v>
+        <v>2021</v>
       </c>
       <c r="C60" t="n">
-        <v>71594594</v>
+        <v>130922410</v>
       </c>
       <c r="D60" t="n">
-        <v>0.0000074949227106673</v>
+        <v>0.000011992586297077</v>
       </c>
       <c r="E60" t="n">
-        <v>13546852</v>
+        <v>-1212889.99999998</v>
       </c>
     </row>
     <row r="61">
       <c r="A61" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="B61" t="n">
-        <v>2021</v>
+        <v>2016</v>
       </c>
       <c r="C61" t="n">
-        <v>65543141</v>
+        <v>96540609</v>
       </c>
       <c r="D61" t="n">
-        <v>0.00000686142274945185</v>
+        <v>0.00000884318876046405</v>
       </c>
       <c r="E61" t="n">
-        <v>1679539</v>
+        <v>9793851</v>
       </c>
     </row>
     <row r="62">
       <c r="A62" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="B62" t="n">
-        <v>2021</v>
+        <v>2016</v>
       </c>
       <c r="C62" t="n">
-        <v>61226578</v>
+        <v>71594594</v>
       </c>
       <c r="D62" t="n">
-        <v>0.00000640954078109085</v>
+        <v>0.00000655811596310509</v>
       </c>
       <c r="E62" t="n">
-        <v>6618937</v>
+        <v>13546852</v>
       </c>
     </row>
     <row r="63">
@@ -1547,15 +1553,83 @@
         <v>46</v>
       </c>
       <c r="B63" t="n">
-        <v>2016</v>
+        <v>2021</v>
       </c>
       <c r="C63" t="n">
+        <v>65543141</v>
+      </c>
+      <c r="D63" t="n">
+        <v>0.00000600379854467989</v>
+      </c>
+      <c r="E63" t="n">
+        <v>1679539</v>
+      </c>
+    </row>
+    <row r="64">
+      <c r="A64" t="s">
+        <v>47</v>
+      </c>
+      <c r="B64" t="n">
+        <v>2021</v>
+      </c>
+      <c r="C64" t="n">
+        <v>63068992</v>
+      </c>
+      <c r="D64" t="n">
+        <v>0.00000577716472855684</v>
+      </c>
+      <c r="E64" t="n">
+        <v>-5800328.00000001</v>
+      </c>
+    </row>
+    <row r="65">
+      <c r="A65" t="s">
+        <v>45</v>
+      </c>
+      <c r="B65" t="n">
+        <v>2021</v>
+      </c>
+      <c r="C65" t="n">
+        <v>61226578</v>
+      </c>
+      <c r="D65" t="n">
+        <v>0.00000560839828979404</v>
+      </c>
+      <c r="E65" t="n">
+        <v>6618937</v>
+      </c>
+    </row>
+    <row r="66">
+      <c r="A66" t="s">
+        <v>46</v>
+      </c>
+      <c r="B66" t="n">
+        <v>2016</v>
+      </c>
+      <c r="C66" t="n">
+        <v>58870176</v>
+      </c>
+      <c r="D66" t="n">
+        <v>0.00000539255018299854</v>
+      </c>
+      <c r="E66" t="n">
+        <v>9890309</v>
+      </c>
+    </row>
+    <row r="67">
+      <c r="A67" t="s">
+        <v>47</v>
+      </c>
+      <c r="B67" t="n">
+        <v>2016</v>
+      </c>
+      <c r="C67" t="n">
         <v>54127984</v>
       </c>
-      <c r="D63" t="n">
-        <v>0.00000566642024067119</v>
-      </c>
-      <c r="E63" t="n">
+      <c r="D67" t="n">
+        <v>0.00000495816200761047</v>
+      </c>
+      <c r="E67" t="n">
         <v>10294644</v>
       </c>
     </row>
@@ -1586,75 +1660,93 @@
       <c r="D1" t="s">
         <v>4</v>
       </c>
+      <c r="E1" t="s">
+        <v>48</v>
+      </c>
     </row>
     <row r="2">
       <c r="A2" t="s">
-        <v>14</v>
+        <v>9</v>
       </c>
       <c r="B2" t="n">
-        <v>161404206940</v>
+        <v>587976000000</v>
       </c>
       <c r="C2" t="n">
-        <v>0.0268545592680974</v>
+        <v>0.0975121230195361</v>
       </c>
       <c r="D2" t="n">
-        <v>45675353140</v>
+        <v>110653248000</v>
+      </c>
+      <c r="E2" t="n">
+        <v>2021</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="s">
-        <v>9</v>
+        <v>6</v>
       </c>
       <c r="B3" t="n">
-        <v>587976000000</v>
+        <v>901490366670</v>
       </c>
       <c r="C3" t="n">
-        <v>0.0978279106819597</v>
+        <v>0.149506509680075</v>
       </c>
       <c r="D3" t="n">
-        <v>110653248000</v>
+        <v>154718673140</v>
+      </c>
+      <c r="E3" t="n">
+        <v>2021</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="s">
-        <v>6</v>
+        <v>12</v>
       </c>
       <c r="B4" t="n">
-        <v>901490366670</v>
+        <v>357816501213</v>
       </c>
       <c r="C4" t="n">
-        <v>0.149990678312108</v>
+        <v>0.0593416171488327</v>
       </c>
       <c r="D4" t="n">
-        <v>154718673140</v>
+        <v>97309179763</v>
+      </c>
+      <c r="E4" t="n">
+        <v>2021</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="B5" t="n">
-        <v>357816501213</v>
+        <v>161404206940</v>
       </c>
       <c r="C5" t="n">
-        <v>0.0595337917214252</v>
+        <v>0.0267678729795161</v>
       </c>
       <c r="D5" t="n">
-        <v>97309179763</v>
+        <v>45675353140</v>
+      </c>
+      <c r="E5" t="n">
+        <v>2021</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="B6" t="n">
-        <v>78963501600</v>
+        <v>98364489600</v>
       </c>
       <c r="C6" t="n">
-        <v>0.0131380096834898</v>
+        <v>0.0163131321867373</v>
       </c>
       <c r="D6" t="n">
-        <v>20951535600</v>
+        <v>28795731600</v>
+      </c>
+      <c r="E6" t="n">
+        <v>2021</v>
       </c>
     </row>
     <row r="7">
@@ -1665,52 +1757,64 @@
         <v>1448217745970</v>
       </c>
       <c r="C7" t="n">
-        <v>0.240955610944634</v>
+        <v>0.240177808284865</v>
       </c>
       <c r="D7" t="n">
         <v>261234414860</v>
       </c>
+      <c r="E7" t="n">
+        <v>2021</v>
+      </c>
     </row>
     <row r="8">
       <c r="A8" t="s">
-        <v>19</v>
+        <v>15</v>
       </c>
       <c r="B8" t="n">
-        <v>52926848000</v>
+        <v>104534296000</v>
       </c>
       <c r="C8" t="n">
-        <v>0.00880601071952198</v>
+        <v>0.0173363557888631</v>
       </c>
       <c r="D8" t="n">
-        <v>12695832000</v>
+        <v>31406700000</v>
+      </c>
+      <c r="E8" t="n">
+        <v>2021</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="s">
-        <v>7</v>
+        <v>22</v>
       </c>
       <c r="B9" t="n">
-        <v>791425215550</v>
+        <v>52926848000</v>
       </c>
       <c r="C9" t="n">
-        <v>0.131677951648156</v>
+        <v>0.00877758499192533</v>
       </c>
       <c r="D9" t="n">
-        <v>49509898210</v>
+        <v>12695832000</v>
+      </c>
+      <c r="E9" t="n">
+        <v>2021</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="s">
-        <v>11</v>
+        <v>7</v>
       </c>
       <c r="B10" t="n">
-        <v>248994048500</v>
+        <v>791425215550</v>
       </c>
       <c r="C10" t="n">
-        <v>0.0414278261986842</v>
+        <v>0.131252896341814</v>
       </c>
       <c r="D10" t="n">
-        <v>7493808500</v>
+        <v>49509898210</v>
+      </c>
+      <c r="E10" t="n">
+        <v>2021</v>
       </c>
     </row>
     <row r="11">
@@ -1718,69 +1822,84 @@
         <v>13</v>
       </c>
       <c r="B11" t="n">
-        <v>231904000000</v>
+        <v>248994048500</v>
       </c>
       <c r="C11" t="n">
-        <v>0.0385843704484353</v>
+        <v>0.04129409752858</v>
       </c>
       <c r="D11" t="n">
-        <v>-28177076000</v>
+        <v>7493808500</v>
+      </c>
+      <c r="E11" t="n">
+        <v>2021</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B12" t="n">
-        <v>131077400000</v>
+        <v>231904000000</v>
       </c>
       <c r="C12" t="n">
-        <v>0.0218087612073001</v>
+        <v>0.0384598204292735</v>
       </c>
       <c r="D12" t="n">
-        <v>-17071064000</v>
+        <v>-28177076000</v>
+      </c>
+      <c r="E12" t="n">
+        <v>2021</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="B13" t="n">
-        <v>52039000000</v>
+        <v>131077400000</v>
       </c>
       <c r="C13" t="n">
-        <v>0.00865828986893768</v>
+        <v>0.021738362711881</v>
       </c>
       <c r="D13" t="n">
-        <v>-7024552000</v>
+        <v>-17071064000</v>
+      </c>
+      <c r="E13" t="n">
+        <v>2021</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="s">
-        <v>16</v>
+        <v>19</v>
       </c>
       <c r="B14" t="n">
-        <v>104534296000</v>
+        <v>97128000000</v>
       </c>
       <c r="C14" t="n">
-        <v>0.0173924986262867</v>
+        <v>0.0161080681603356</v>
       </c>
       <c r="D14" t="n">
-        <v>31406700000</v>
+        <v>-13019696000</v>
+      </c>
+      <c r="E14" t="n">
+        <v>2021</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="s">
-        <v>18</v>
+        <v>21</v>
       </c>
       <c r="B15" t="n">
         <v>59395150000</v>
       </c>
       <c r="C15" t="n">
-        <v>0.00988221190855001</v>
+        <v>0.00985031221268181</v>
       </c>
       <c r="D15" t="n">
         <v>2321468000</v>
+      </c>
+      <c r="E15" t="n">
+        <v>2021</v>
       </c>
     </row>
     <row r="16">
@@ -1791,24 +1910,30 @@
         <v>649806185770</v>
       </c>
       <c r="C16" t="n">
-        <v>0.108115265762705</v>
+        <v>0.107766270605705</v>
       </c>
       <c r="D16" t="n">
         <v>160198525120</v>
       </c>
+      <c r="E16" t="n">
+        <v>2021</v>
+      </c>
     </row>
     <row r="17">
       <c r="A17" t="s">
-        <v>47</v>
+        <v>49</v>
       </c>
       <c r="B17" t="n">
-        <v>152338819769</v>
+        <v>107312888761</v>
       </c>
       <c r="C17" t="n">
-        <v>0.025346252999709</v>
+        <v>0.0177971679293788</v>
       </c>
       <c r="D17" t="n">
-        <v>9061756803</v>
+        <v>15051100475</v>
+      </c>
+      <c r="E17" t="n">
+        <v>2021</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
change conduent to buck and edit plots
</commit_message>
<xml_diff>
--- a/Actuarial Firm Summary.xlsx
+++ b/Actuarial Firm Summary.xlsx
@@ -13,7 +13,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="50">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="47" uniqueCount="47">
   <si>
     <t xml:space="preserve">actuarial_firm_name</t>
   </si>
@@ -45,10 +45,7 @@
     <t xml:space="preserve">CalPERS</t>
   </si>
   <si>
-    <t xml:space="preserve">Scott Terando</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Conduent (formerly Buck and/or Xerox)</t>
+    <t xml:space="preserve">Buck</t>
   </si>
   <si>
     <t xml:space="preserve">Cheiron</t>
@@ -60,24 +57,21 @@
     <t xml:space="preserve">New York State and Local Retirement Systems' Actuary</t>
   </si>
   <si>
-    <t xml:space="preserve">Internal Actuarial Services</t>
-  </si>
-  <si>
     <t xml:space="preserve">New York State And Local Retirement Systems' Actuary</t>
   </si>
   <si>
     <t xml:space="preserve">Nystrs Office Of The Actuary</t>
   </si>
   <si>
+    <t xml:space="preserve">Public Employee Retirement Administration Commission</t>
+  </si>
+  <si>
     <t xml:space="preserve">Foster &amp; Foster</t>
   </si>
   <si>
     <t xml:space="preserve">Office of The State Actuary - Washington</t>
   </si>
   <si>
-    <t xml:space="preserve">Perac</t>
-  </si>
-  <si>
     <t xml:space="preserve">Pwc</t>
   </si>
   <si>
@@ -148,9 +142,6 @@
   </si>
   <si>
     <t xml:space="preserve">Arthur J. Gallagher &amp; Co.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Usi Consulting Group</t>
   </si>
   <si>
     <t xml:space="preserve">Principal Financial Group</t>
@@ -666,7 +657,7 @@
     </row>
     <row r="11">
       <c r="A11" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B11" t="n">
         <v>2016</v>
@@ -683,7 +674,7 @@
     </row>
     <row r="12">
       <c r="A12" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B12" t="n">
         <v>2016</v>
@@ -700,7 +691,7 @@
     </row>
     <row r="13">
       <c r="A13" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B13" t="n">
         <v>2021</v>
@@ -717,7 +708,7 @@
     </row>
     <row r="14">
       <c r="A14" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B14" t="n">
         <v>2021</v>
@@ -734,7 +725,7 @@
     </row>
     <row r="15">
       <c r="A15" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B15" t="n">
         <v>2021</v>
@@ -751,7 +742,7 @@
     </row>
     <row r="16">
       <c r="A16" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="B16" t="n">
         <v>2016</v>
@@ -768,7 +759,7 @@
     </row>
     <row r="17">
       <c r="A17" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="B17" t="n">
         <v>2016</v>
@@ -785,7 +776,7 @@
     </row>
     <row r="18">
       <c r="A18" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B18" t="n">
         <v>2021</v>
@@ -802,7 +793,7 @@
     </row>
     <row r="19">
       <c r="A19" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="B19" t="n">
         <v>2021</v>
@@ -819,7 +810,7 @@
     </row>
     <row r="20">
       <c r="A20" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="B20" t="n">
         <v>2016</v>
@@ -836,7 +827,7 @@
     </row>
     <row r="21">
       <c r="A21" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="B21" t="n">
         <v>2021</v>
@@ -853,7 +844,7 @@
     </row>
     <row r="22">
       <c r="A22" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B22" t="n">
         <v>2021</v>
@@ -870,7 +861,7 @@
     </row>
     <row r="23">
       <c r="A23" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B23" t="n">
         <v>2021</v>
@@ -887,7 +878,7 @@
     </row>
     <row r="24">
       <c r="A24" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B24" t="n">
         <v>2016</v>
@@ -904,7 +895,7 @@
     </row>
     <row r="25">
       <c r="A25" t="s">
-        <v>20</v>
+        <v>16</v>
       </c>
       <c r="B25" t="n">
         <v>2016</v>
@@ -921,7 +912,7 @@
     </row>
     <row r="26">
       <c r="A26" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="B26" t="n">
         <v>2016</v>
@@ -938,7 +929,7 @@
     </row>
     <row r="27">
       <c r="A27" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B27" t="n">
         <v>2016</v>
@@ -955,7 +946,7 @@
     </row>
     <row r="28">
       <c r="A28" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="B28" t="n">
         <v>2021</v>
@@ -972,7 +963,7 @@
     </row>
     <row r="29">
       <c r="A29" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="B29" t="n">
         <v>2021</v>
@@ -989,7 +980,7 @@
     </row>
     <row r="30">
       <c r="A30" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="B30" t="n">
         <v>2016</v>
@@ -1006,7 +997,7 @@
     </row>
     <row r="31">
       <c r="A31" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="B31" t="n">
         <v>2016</v>
@@ -1023,24 +1014,24 @@
     </row>
     <row r="32">
       <c r="A32" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="B32" t="n">
         <v>2021</v>
       </c>
       <c r="C32" t="n">
-        <v>45250140000</v>
+        <v>45311366578</v>
       </c>
       <c r="D32" t="n">
-        <v>0.00414494515419335</v>
+        <v>0.00415055355248314</v>
       </c>
       <c r="E32" t="n">
-        <v>13589248000</v>
+        <v>13595866937</v>
       </c>
     </row>
     <row r="33">
       <c r="A33" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="B33" t="n">
         <v>2016</v>
@@ -1057,7 +1048,7 @@
     </row>
     <row r="34">
       <c r="A34" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="B34" t="n">
         <v>2016</v>
@@ -1074,7 +1065,7 @@
     </row>
     <row r="35">
       <c r="A35" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B35" t="n">
         <v>2016</v>
@@ -1091,7 +1082,7 @@
     </row>
     <row r="36">
       <c r="A36" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="B36" t="n">
         <v>2021</v>
@@ -1108,7 +1099,7 @@
     </row>
     <row r="37">
       <c r="A37" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="B37" t="n">
         <v>2016</v>
@@ -1125,7 +1116,7 @@
     </row>
     <row r="38">
       <c r="A38" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="B38" t="n">
         <v>2021</v>
@@ -1142,7 +1133,7 @@
     </row>
     <row r="39">
       <c r="A39" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="B39" t="n">
         <v>2016</v>
@@ -1159,7 +1150,7 @@
     </row>
     <row r="40">
       <c r="A40" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="B40" t="n">
         <v>2021</v>
@@ -1176,7 +1167,7 @@
     </row>
     <row r="41">
       <c r="A41" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="B41" t="n">
         <v>2016</v>
@@ -1193,7 +1184,7 @@
     </row>
     <row r="42">
       <c r="A42" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="B42" t="n">
         <v>2021</v>
@@ -1210,7 +1201,7 @@
     </row>
     <row r="43">
       <c r="A43" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="B43" t="n">
         <v>2021</v>
@@ -1227,7 +1218,7 @@
     </row>
     <row r="44">
       <c r="A44" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="B44" t="n">
         <v>2021</v>
@@ -1244,7 +1235,7 @@
     </row>
     <row r="45">
       <c r="A45" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="B45" t="n">
         <v>2021</v>
@@ -1261,7 +1252,7 @@
     </row>
     <row r="46">
       <c r="A46" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="B46" t="n">
         <v>2021</v>
@@ -1278,7 +1269,7 @@
     </row>
     <row r="47">
       <c r="A47" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="B47" t="n">
         <v>2016</v>
@@ -1295,7 +1286,7 @@
     </row>
     <row r="48">
       <c r="A48" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="B48" t="n">
         <v>2016</v>
@@ -1312,7 +1303,7 @@
     </row>
     <row r="49">
       <c r="A49" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="B49" t="n">
         <v>2016</v>
@@ -1329,7 +1320,7 @@
     </row>
     <row r="50">
       <c r="A50" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="B50" t="n">
         <v>2021</v>
@@ -1346,7 +1337,7 @@
     </row>
     <row r="51">
       <c r="A51" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="B51" t="n">
         <v>2021</v>
@@ -1363,7 +1354,7 @@
     </row>
     <row r="52">
       <c r="A52" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="B52" t="n">
         <v>2016</v>
@@ -1380,7 +1371,7 @@
     </row>
     <row r="53">
       <c r="A53" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="B53" t="n">
         <v>2021</v>
@@ -1397,7 +1388,7 @@
     </row>
     <row r="54">
       <c r="A54" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="B54" t="n">
         <v>2016</v>
@@ -1414,7 +1405,7 @@
     </row>
     <row r="55">
       <c r="A55" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="B55" t="n">
         <v>2021</v>
@@ -1431,7 +1422,7 @@
     </row>
     <row r="56">
       <c r="A56" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="B56" t="n">
         <v>2021</v>
@@ -1448,7 +1439,7 @@
     </row>
     <row r="57">
       <c r="A57" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="B57" t="n">
         <v>2016</v>
@@ -1465,7 +1456,7 @@
     </row>
     <row r="58">
       <c r="A58" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="B58" t="n">
         <v>2016</v>
@@ -1482,7 +1473,7 @@
     </row>
     <row r="59">
       <c r="A59" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="B59" t="n">
         <v>2016</v>
@@ -1499,7 +1490,7 @@
     </row>
     <row r="60">
       <c r="A60" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="B60" t="n">
         <v>2021</v>
@@ -1516,7 +1507,7 @@
     </row>
     <row r="61">
       <c r="A61" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="B61" t="n">
         <v>2016</v>
@@ -1533,7 +1524,7 @@
     </row>
     <row r="62">
       <c r="A62" t="s">
-        <v>45</v>
+        <v>22</v>
       </c>
       <c r="B62" t="n">
         <v>2016</v>
@@ -1550,7 +1541,7 @@
     </row>
     <row r="63">
       <c r="A63" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
       <c r="B63" t="n">
         <v>2021</v>
@@ -1567,7 +1558,7 @@
     </row>
     <row r="64">
       <c r="A64" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
       <c r="B64" t="n">
         <v>2021</v>
@@ -1584,52 +1575,35 @@
     </row>
     <row r="65">
       <c r="A65" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="B65" t="n">
-        <v>2021</v>
+        <v>2016</v>
       </c>
       <c r="C65" t="n">
-        <v>61226578</v>
+        <v>58870176</v>
       </c>
       <c r="D65" t="n">
-        <v>0.00000560839828979404</v>
+        <v>0.00000539255018299854</v>
       </c>
       <c r="E65" t="n">
-        <v>6618937</v>
+        <v>9890309</v>
       </c>
     </row>
     <row r="66">
       <c r="A66" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="B66" t="n">
         <v>2016</v>
       </c>
       <c r="C66" t="n">
-        <v>58870176</v>
+        <v>54127984</v>
       </c>
       <c r="D66" t="n">
-        <v>0.00000539255018299854</v>
+        <v>0.00000495816200761047</v>
       </c>
       <c r="E66" t="n">
-        <v>9890309</v>
-      </c>
-    </row>
-    <row r="67">
-      <c r="A67" t="s">
-        <v>47</v>
-      </c>
-      <c r="B67" t="n">
-        <v>2016</v>
-      </c>
-      <c r="C67" t="n">
-        <v>54127984</v>
-      </c>
-      <c r="D67" t="n">
-        <v>0.00000495816200761047</v>
-      </c>
-      <c r="E67" t="n">
         <v>10294644</v>
       </c>
     </row>
@@ -1661,21 +1635,21 @@
         <v>4</v>
       </c>
       <c r="E1" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="B2" t="n">
-        <v>587976000000</v>
+        <v>161404206940</v>
       </c>
       <c r="C2" t="n">
-        <v>0.0975121230195361</v>
+        <v>0.0267678729795161</v>
       </c>
       <c r="D2" t="n">
-        <v>110653248000</v>
+        <v>45675353140</v>
       </c>
       <c r="E2" t="n">
         <v>2021</v>
@@ -1683,16 +1657,16 @@
     </row>
     <row r="3">
       <c r="A3" t="s">
-        <v>6</v>
+        <v>9</v>
       </c>
       <c r="B3" t="n">
-        <v>901490366670</v>
+        <v>587976000000</v>
       </c>
       <c r="C3" t="n">
-        <v>0.149506509680075</v>
+        <v>0.0975121230195361</v>
       </c>
       <c r="D3" t="n">
-        <v>154718673140</v>
+        <v>110653248000</v>
       </c>
       <c r="E3" t="n">
         <v>2021</v>
@@ -1700,16 +1674,16 @@
     </row>
     <row r="4">
       <c r="A4" t="s">
-        <v>12</v>
+        <v>6</v>
       </c>
       <c r="B4" t="n">
-        <v>357816501213</v>
+        <v>901490366670</v>
       </c>
       <c r="C4" t="n">
-        <v>0.0593416171488327</v>
+        <v>0.149506509680075</v>
       </c>
       <c r="D4" t="n">
-        <v>97309179763</v>
+        <v>154718673140</v>
       </c>
       <c r="E4" t="n">
         <v>2021</v>
@@ -1720,13 +1694,13 @@
         <v>11</v>
       </c>
       <c r="B5" t="n">
-        <v>161404206940</v>
+        <v>357816501213</v>
       </c>
       <c r="C5" t="n">
-        <v>0.0267678729795161</v>
+        <v>0.0593416171488327</v>
       </c>
       <c r="D5" t="n">
-        <v>45675353140</v>
+        <v>97309179763</v>
       </c>
       <c r="E5" t="n">
         <v>2021</v>
@@ -1734,7 +1708,7 @@
     </row>
     <row r="6">
       <c r="A6" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B6" t="n">
         <v>98364489600</v>
@@ -1768,16 +1742,16 @@
     </row>
     <row r="8">
       <c r="A8" t="s">
-        <v>15</v>
+        <v>20</v>
       </c>
       <c r="B8" t="n">
-        <v>104534296000</v>
+        <v>52926848000</v>
       </c>
       <c r="C8" t="n">
-        <v>0.0173363557888631</v>
+        <v>0.00877758499192533</v>
       </c>
       <c r="D8" t="n">
-        <v>31406700000</v>
+        <v>12695832000</v>
       </c>
       <c r="E8" t="n">
         <v>2021</v>
@@ -1785,16 +1759,16 @@
     </row>
     <row r="9">
       <c r="A9" t="s">
-        <v>22</v>
+        <v>7</v>
       </c>
       <c r="B9" t="n">
-        <v>52926848000</v>
+        <v>791425215550</v>
       </c>
       <c r="C9" t="n">
-        <v>0.00877758499192533</v>
+        <v>0.131252896341814</v>
       </c>
       <c r="D9" t="n">
-        <v>12695832000</v>
+        <v>49509898210</v>
       </c>
       <c r="E9" t="n">
         <v>2021</v>
@@ -1802,16 +1776,16 @@
     </row>
     <row r="10">
       <c r="A10" t="s">
-        <v>7</v>
+        <v>12</v>
       </c>
       <c r="B10" t="n">
-        <v>791425215550</v>
+        <v>248994048500</v>
       </c>
       <c r="C10" t="n">
-        <v>0.131252896341814</v>
+        <v>0.04129409752858</v>
       </c>
       <c r="D10" t="n">
-        <v>49509898210</v>
+        <v>7493808500</v>
       </c>
       <c r="E10" t="n">
         <v>2021</v>
@@ -1822,13 +1796,13 @@
         <v>13</v>
       </c>
       <c r="B11" t="n">
-        <v>248994048500</v>
+        <v>231904000000</v>
       </c>
       <c r="C11" t="n">
-        <v>0.04129409752858</v>
+        <v>0.0384598204292735</v>
       </c>
       <c r="D11" t="n">
-        <v>7493808500</v>
+        <v>-28177076000</v>
       </c>
       <c r="E11" t="n">
         <v>2021</v>
@@ -1836,16 +1810,16 @@
     </row>
     <row r="12">
       <c r="A12" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="B12" t="n">
-        <v>231904000000</v>
+        <v>131077400000</v>
       </c>
       <c r="C12" t="n">
-        <v>0.0384598204292735</v>
+        <v>0.021738362711881</v>
       </c>
       <c r="D12" t="n">
-        <v>-28177076000</v>
+        <v>-17071064000</v>
       </c>
       <c r="E12" t="n">
         <v>2021</v>
@@ -1853,16 +1827,16 @@
     </row>
     <row r="13">
       <c r="A13" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="B13" t="n">
-        <v>131077400000</v>
+        <v>97128000000</v>
       </c>
       <c r="C13" t="n">
-        <v>0.021738362711881</v>
+        <v>0.0161080681603356</v>
       </c>
       <c r="D13" t="n">
-        <v>-17071064000</v>
+        <v>-13019696000</v>
       </c>
       <c r="E13" t="n">
         <v>2021</v>
@@ -1870,16 +1844,16 @@
     </row>
     <row r="14">
       <c r="A14" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="B14" t="n">
-        <v>97128000000</v>
+        <v>104534296000</v>
       </c>
       <c r="C14" t="n">
-        <v>0.0161080681603356</v>
+        <v>0.0173363557888631</v>
       </c>
       <c r="D14" t="n">
-        <v>-13019696000</v>
+        <v>31406700000</v>
       </c>
       <c r="E14" t="n">
         <v>2021</v>
@@ -1887,7 +1861,7 @@
     </row>
     <row r="15">
       <c r="A15" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="B15" t="n">
         <v>59395150000</v>
@@ -1921,7 +1895,7 @@
     </row>
     <row r="17">
       <c r="A17" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
       <c r="B17" t="n">
         <v>107312888761</v>

</xml_diff>